<commit_message>
adding testng.xml into project
</commit_message>
<xml_diff>
--- a/Resources/Data.xlsx
+++ b/Resources/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="4950"/>
   </bookViews>
   <sheets>
     <sheet name="MemberDetails" sheetId="1" r:id="rId1"/>
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adding to member payment
</commit_message>
<xml_diff>
--- a/Resources/Data.xlsx
+++ b/Resources/Data.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="3495" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="3495"/>
   </bookViews>
   <sheets>
     <sheet name="MemberDetails" sheetId="1" r:id="rId1"/>
     <sheet name="UserAccountTypes" sheetId="2" r:id="rId2"/>
-    <sheet name="TRANSACTION_DATA" sheetId="3" r:id="rId3"/>
+    <sheet name="TransactionData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
   <si>
     <t>Savings Account</t>
   </si>
@@ -208,6 +208,18 @@
   </si>
   <si>
     <t>TXN010</t>
+  </si>
+  <si>
+    <t>Savings to Current</t>
+  </si>
+  <si>
+    <t>Miscellaneous Expenses</t>
+  </si>
+  <si>
+    <t>MEM006</t>
+  </si>
+  <si>
+    <t>TestUser41</t>
   </si>
 </sst>
 </file>
@@ -607,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,6 +888,44 @@
         <v>44</v>
       </c>
     </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2">
+        <v>33188</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7">
+        <v>570012</v>
+      </c>
+      <c r="J7">
+        <v>9879879870</v>
+      </c>
+      <c r="K7">
+        <v>2813928232</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1"/>
@@ -883,6 +933,7 @@
     <hyperlink ref="L4" r:id="rId3"/>
     <hyperlink ref="L5" r:id="rId4"/>
     <hyperlink ref="L6" r:id="rId5"/>
+    <hyperlink ref="L7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -951,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,6 +1036,15 @@
       <c r="A2" s="5" t="s">
         <v>54</v>
       </c>
+      <c r="B2" s="5">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">

</xml_diff>

<commit_message>
member payment confirmation page object
</commit_message>
<xml_diff>
--- a/Resources/Data.xlsx
+++ b/Resources/Data.xlsx
@@ -4,20 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="3255" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="3495"/>
   </bookViews>
   <sheets>
     <sheet name="MemberDetails" sheetId="1" r:id="rId1"/>
     <sheet name="UserAccountTypes" sheetId="2" r:id="rId2"/>
-    <sheet name="MemberPayment" sheetId="3" r:id="rId3"/>
+    <sheet name="TransactionData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J8"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
   <si>
     <t>Savings Account</t>
   </si>
@@ -163,38 +162,71 @@
     <t>admin@gmail.com</t>
   </si>
   <si>
+    <t>MEM005</t>
+  </si>
+  <si>
+    <t>TestUser40</t>
+  </si>
+  <si>
+    <t>TRANSACTION_AMOUNT</t>
+  </si>
+  <si>
+    <t>TRANSACTION_TYPE</t>
+  </si>
+  <si>
+    <t>TRANSACTION_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>SUBMITTED_AT</t>
+  </si>
+  <si>
     <t>TXN001</t>
   </si>
   <si>
-    <t>Transaction_Name</t>
-  </si>
-  <si>
-    <t>Transaction_Login</t>
-  </si>
-  <si>
-    <t>Transaction_Type</t>
-  </si>
-  <si>
-    <t>Transaction_Amount</t>
-  </si>
-  <si>
-    <t>Transaction_Description</t>
+    <t>TXN002</t>
+  </si>
+  <si>
+    <t>TXN003</t>
+  </si>
+  <si>
+    <t>TXN004</t>
+  </si>
+  <si>
+    <t>TXN005</t>
+  </si>
+  <si>
+    <t>TXN006</t>
+  </si>
+  <si>
+    <t>TXN007</t>
+  </si>
+  <si>
+    <t>TXN008</t>
+  </si>
+  <si>
+    <t>TXN009</t>
+  </si>
+  <si>
+    <t>TXN010</t>
   </si>
   <si>
     <t>Savings to Current</t>
   </si>
   <si>
-    <t>Miscellaneous Expense</t>
-  </si>
-  <si>
-    <t>TestUser01</t>
+    <t>Miscellaneous Expenses</t>
+  </si>
+  <si>
+    <t>MEM006</t>
+  </si>
+  <si>
+    <t>TestUser41</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +246,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -261,14 +301,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -574,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,12 +850,90 @@
         <v>47</v>
       </c>
     </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2">
+        <v>33188</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6">
+        <v>570012</v>
+      </c>
+      <c r="J6">
+        <v>9879879870</v>
+      </c>
+      <c r="K6">
+        <v>2813928232</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2">
+        <v>33188</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7">
+        <v>570012</v>
+      </c>
+      <c r="J7">
+        <v>9879879870</v>
+      </c>
+      <c r="K7">
+        <v>2813928232</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1"/>
     <hyperlink ref="L3" r:id="rId2"/>
     <hyperlink ref="L4" r:id="rId3"/>
     <hyperlink ref="L5" r:id="rId4"/>
+    <hyperlink ref="L6" r:id="rId5"/>
+    <hyperlink ref="L7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -821,7 +944,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,23 +1000,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="19" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="27" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -901,41 +1023,78 @@
         <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>52</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="5">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="4">
-        <v>534</v>
-      </c>
-      <c r="E2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25"/>
+      <c r="B4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>